<commit_message>
Delta Processor : Add Cleaning DeltaIndicator Column Function
</commit_message>
<xml_diff>
--- a/Master4.xlsx
+++ b/Master4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/j_a_vorathammaporn_accenture_com/Documents/Desktop/PTT-WorkSpace/Accenture-Data-Migration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{AFCA3FCF-CF0C-4C99-846F-13DADE525259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4D87100-6BE2-4015-A4B6-54275A25994C}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{AFCA3FCF-CF0C-4C99-846F-13DADE525259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F6A8B84-FBA4-4A84-A478-E8CC640DC9A4}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5553D876-8CE6-4031-8D37-2253051AB329}"/>
+    <workbookView xWindow="-5520" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{5553D876-8CE6-4031-8D37-2253051AB329}"/>
   </bookViews>
   <sheets>
     <sheet name="File List" sheetId="1" r:id="rId1"/>
@@ -118,7 +118,7 @@
     <t>C:\Users\j.a.vorathammaporn\OneDrive - Accenture\Desktop\PTT-WorkSpace\SandBox\DeltaTest\Python_Result\</t>
   </si>
   <si>
-    <t>BeforeDelta_Python.xlsx</t>
+    <t>BeforeDelta_Python_MOCK4.xlsx</t>
   </si>
 </sst>
 </file>
@@ -298,13 +298,13 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
+          <xdr:colOff>15240</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>63500</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -336,7 +336,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="73152" tIns="73152" rIns="73152" bIns="73152" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="64008" tIns="64008" rIns="64008" bIns="64008" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -373,13 +373,13 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
+          <xdr:colOff>15240</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>63500</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -411,7 +411,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="73152" tIns="73152" rIns="73152" bIns="73152" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="64008" tIns="64008" rIns="64008" bIns="64008" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -448,13 +448,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>63500</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -486,7 +486,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="73152" tIns="73152" rIns="73152" bIns="73152" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="64008" tIns="64008" rIns="64008" bIns="64008" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -835,18 +835,18 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="58.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="58.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.81640625" customWidth="1"/>
-    <col min="2" max="2" width="33.36328125" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875"/>
-    <col min="4" max="4" width="61.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.77734375" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.21875"/>
+    <col min="4" max="4" width="61.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -854,7 +854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="39" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" ht="41.4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -865,31 +865,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
     </row>
@@ -910,13 +910,13 @@
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>177800</xdr:rowOff>
+                    <xdr:rowOff>175260</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>12700</xdr:colOff>
+                    <xdr:colOff>15240</xdr:colOff>
                     <xdr:row>13</xdr:row>
-                    <xdr:rowOff>63500</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -938,12 +938,12 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="61.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="61.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="6:6" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="6:6" ht="18" x14ac:dyDescent="0.35">
       <c r="F5" s="6" t="s">
         <v>2</v>
       </c>
@@ -964,13 +964,13 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>177800</xdr:rowOff>
+                    <xdr:rowOff>175260</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>6</xdr:col>
-                    <xdr:colOff>12700</xdr:colOff>
+                    <xdr:colOff>15240</xdr:colOff>
                     <xdr:row>16</xdr:row>
-                    <xdr:rowOff>63500</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -992,13 +992,13 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="22.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="83.90625" customWidth="1"/>
+    <col min="3" max="3" width="83.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1007,7 +1007,7 @@
       </c>
       <c r="C1" s="8"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -1025,7 +1025,7 @@
       </c>
       <c r="C3" s="9"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -1034,7 +1034,7 @@
       </c>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -1052,7 +1052,7 @@
       </c>
       <c r="C6" s="9"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="C7" s="9"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1070,7 +1070,7 @@
       </c>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="C9" s="10"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1102,18 +1102,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1137,13 +1137,13 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>177800</xdr:rowOff>
+                    <xdr:rowOff>175260</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>13</xdr:row>
-                    <xdr:rowOff>63500</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1165,14 +1165,14 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="22.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -1183,6 +1183,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009796AFA9FB23BA42968688ABCE634A9C" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f5a84ed632dcf9c8f7b4d62f9d6a102e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2f423150-2cdd-48d9-9270-a69c1f7e699a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="19a6001113795a3bb37fd59fb77570ff" ns2:_="">
     <xsd:import namespace="2f423150-2cdd-48d9-9270-a69c1f7e699a"/>
@@ -1320,22 +1335,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A630574-B6C5-4FE9-AFE1-1071C5FE6BAC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9dd6596e-c8f8-4455-8ee4-66d436aee8c7"/>
+    <ds:schemaRef ds:uri="e4f4844b-0fda-4019-a303-3beba8e8a91a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{372C0842-4D4A-446D-8B45-AE815A5DAA02}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D3FBD79-3017-4DAB-9132-325B92A4D8A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1353,25 +1372,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{372C0842-4D4A-446D-8B45-AE815A5DAA02}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A630574-B6C5-4FE9-AFE1-1071C5FE6BAC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9dd6596e-c8f8-4455-8ee4-66d436aee8c7"/>
-    <ds:schemaRef ds:uri="e4f4844b-0fda-4019-a303-3beba8e8a91a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>